<commit_message>
Homelessness text correction and housing graph y axis padding.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_uploader/housing_homelessness.xlsx
+++ b/dashboard_loader/housing_homelessness_uploader/housing_homelessness.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t xml:space="preserve">Number of people who were homeless, by state and territory, 2006, 2011 and 2016</t>
   </si>
@@ -92,7 +92,10 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">The number of homeless persons was over 116,000 in 2016 – a 29.8 per cent increase from just under 90,000 in 2006 and a 13.7 per cent increase from 102,000 in 2011. This is around 50 homeless for every 10,000 people. The benchmark was not met.</t>
+    <t xml:space="preserve">The number of homeless persons was over 116,000 in 2016 – a 29.8 per cent increase from just under 90,000 in 2006 and a 13.7 per cent increase from 102,000 in 2011. The national benchmark was not met.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State and Territory assessments are made against the agreed performance indicator — proportion of Australians who are homeless. This was around 50 homeless for every 10,000 people nationally in 2016</t>
   </si>
   <si>
     <t xml:space="preserve">Most of the increase in homelessness between was reflected in people living in 'severely' crowded dwellings, up from 31,531 in 2006 and 41,370 in 2011 to 51,088 in 2016 (ABS 2018).</t>
@@ -736,10 +739,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -781,7 +784,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
@@ -789,46 +792,51 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>